<commit_message>
[DataTable] FarmerStatTable -> FarmerLevelTable로 마이그레이션 & 테이블 정리
</commit_message>
<xml_diff>
--- a/DataTable/AdventureCropLootTable.xlsx
+++ b/DataTable/AdventureCropLootTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seh00n/GitHub/ProjectF/DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C8B98749-76C6-724E-9D05-461E3DCF195B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CCDE9EC9-34AD-2F42-86EC-A5F9CFEF793F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2940" yWindow="2120" windowWidth="28300" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1050,7 +1050,10 @@
   <dimension ref="A2:F273"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B273" sqref="B273"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>

</xml_diff>